<commit_message>
Progress on calculating neighbors
</commit_message>
<xml_diff>
--- a/minesweeper/algorithm.xlsx
+++ b/minesweeper/algorithm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelgodfreysmith/Projects/exercism/rust/minesweeper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF9D65C-A26A-E74E-A19C-B3DE638D46F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE24714C-8569-684C-91DF-79B94DD0B712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{E053F562-A7B4-7F4D-B209-B696D6BAF78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{E053F562-A7B4-7F4D-B209-B696D6BAF78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>n-1</t>
   </si>
@@ -60,6 +60,48 @@
   </si>
   <si>
     <t>5. Construct a new board with the "*" and the sum of the neighbor points at the correct indices</t>
+  </si>
+  <si>
+    <t>(r-1, c-1)</t>
+  </si>
+  <si>
+    <t>* (r, c)</t>
+  </si>
+  <si>
+    <t>(r-1, c)</t>
+  </si>
+  <si>
+    <t>(r-1, c+1)</t>
+  </si>
+  <si>
+    <t>(r, c-1)</t>
+  </si>
+  <si>
+    <t>(r, c+1)</t>
+  </si>
+  <si>
+    <t>(r+1, c-1)</t>
+  </si>
+  <si>
+    <t>(r+1, c)</t>
+  </si>
+  <si>
+    <t>(r+1, c+1)</t>
+  </si>
+  <si>
+    <t>Calculate potnetial neighbors of (r, c)</t>
+  </si>
+  <si>
+    <t>1) r of neighbor must be &lt;= row len</t>
+  </si>
+  <si>
+    <t>2) c of neighbor must be &lt;= column len</t>
+  </si>
+  <si>
+    <t>Rules to validate neighbor points</t>
+  </si>
+  <si>
+    <t>3) other mines don't count as neighbors</t>
   </si>
 </sst>
 </file>
@@ -432,15 +474,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F537145F-1469-D14C-8241-6CF0D920BED5}">
-  <dimension ref="A2:J20"/>
+  <dimension ref="A2:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>0</v>
@@ -461,7 +503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -475,7 +517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -489,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -503,7 +545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -519,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -535,7 +577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -549,7 +591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -560,7 +602,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -571,7 +613,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -582,7 +624,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -593,7 +635,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -603,43 +645,92 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -649,8 +740,14 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -660,8 +757,14 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,8 +774,29 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="J21" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working on logic to reject neighbors outside the grid boundaries
</commit_message>
<xml_diff>
--- a/minesweeper/algorithm.xlsx
+++ b/minesweeper/algorithm.xlsx
@@ -1,119 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelgodfreysmith/Projects/exercism/rust/minesweeper/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE24714C-8569-684C-91DF-79B94DD0B712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{E053F562-A7B4-7F4D-B209-B696D6BAF78E}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>n-1</t>
   </si>
   <si>
+    <t xml:space="preserve">1. Convert input (array of strings) to a 2D array of chars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Search each cell of the 2D array for "*"s and record their indices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. For each "*" point, calculate it's neighbor indices</t>
+  </si>
+  <si>
     <t>*</t>
   </si>
   <si>
-    <t>1. Convert input (array of strings) to a 2D array of chars</t>
-  </si>
-  <si>
-    <t>6. Convert the board to the proper output type</t>
-  </si>
-  <si>
-    <t>2. Search each cell of the 2D array for "*"s and record their indices</t>
-  </si>
-  <si>
-    <t>3. For each "*" point, calculate it's neighbor indices</t>
-  </si>
-  <si>
-    <t>4. Add up the count of overlapping neighbor points</t>
-  </si>
-  <si>
-    <t>5. Construct a new board with the "*" and the sum of the neighbor points at the correct indices</t>
-  </si>
-  <si>
-    <t>(r-1, c-1)</t>
-  </si>
-  <si>
-    <t>* (r, c)</t>
-  </si>
-  <si>
-    <t>(r-1, c)</t>
-  </si>
-  <si>
-    <t>(r-1, c+1)</t>
-  </si>
-  <si>
-    <t>(r, c-1)</t>
-  </si>
-  <si>
-    <t>(r, c+1)</t>
-  </si>
-  <si>
-    <t>(r+1, c-1)</t>
-  </si>
-  <si>
-    <t>(r+1, c)</t>
-  </si>
-  <si>
-    <t>(r+1, c+1)</t>
-  </si>
-  <si>
-    <t>Calculate potnetial neighbors of (r, c)</t>
-  </si>
-  <si>
-    <t>1) r of neighbor must be &lt;= row len</t>
-  </si>
-  <si>
-    <t>2) c of neighbor must be &lt;= column len</t>
-  </si>
-  <si>
-    <t>Rules to validate neighbor points</t>
-  </si>
-  <si>
-    <t>3) other mines don't count as neighbors</t>
+    <t xml:space="preserve">4. Add up the count of overlapping neighbor points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Construct a new board with the "*" and the sum of the neighbor points at the correct indices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Convert the board to the proper output type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate potnetial neighbors of (r, c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rules to validate neighbor points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(r-1, c-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(r-1, c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(r-1, c+1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) r of neighbor must be &gt;=0 and &lt;= (row len - 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(r, c-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* (r, c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(r, c+1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2) c of neighbor must be &gt;=0 and &lt;= (column len -1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(r+1, c-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(r+1, c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(r+1, c+1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3) other mines don't count as neighbors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
-      <sz val="12"/>
+      <name val="Calibri"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="12.000000"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -150,14 +126,14 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -170,15 +146,295 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -220,108 +476,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -329,7 +491,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -355,7 +517,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -407,16 +569,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -432,7 +606,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -463,26 +637,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F537145F-1469-D14C-8241-6CF0D920BED5}">
-  <dimension ref="A2:N21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="O28" activeCellId="0" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" ht="17">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>0</v>
@@ -503,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" ht="18">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -514,10 +681,10 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="J3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="18">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -528,10 +695,10 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="J4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" ht="18">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -542,42 +709,42 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="J5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" ht="18">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="J6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" ht="18">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="J7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" ht="18">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -588,10 +755,10 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="J8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" ht="18">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -602,7 +769,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" ht="18">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -613,7 +780,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" ht="18">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -624,7 +791,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" ht="18">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -635,7 +802,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" ht="18">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -646,13 +813,13 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="N13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" ht="18">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -660,25 +827,25 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" ht="18">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -686,25 +853,25 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" ht="18">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -712,25 +879,25 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I16">
         <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" ht="18">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -744,10 +911,10 @@
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" ht="18">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -761,10 +928,10 @@
         <v>5</v>
       </c>
       <c r="J18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" ht="18">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -778,26 +945,32 @@
         <v>6</v>
       </c>
       <c r="J19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" ht="17">
       <c r="I20">
         <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="I21">
         <v>8</v>
       </c>
       <c r="J21" t="s">
-        <v>16</v>
-      </c>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" ht="16.5">
+      <c r="N24"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>